<commit_message>
Add AddCourse and RegisterCourse
</commit_message>
<xml_diff>
--- a/ExcelProject/Register Student.xlsx
+++ b/ExcelProject/Register Student.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalem\OneDrive\Desktop\Project_Test_Tutors\ExcelProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0176DA02-7D8A-4768-B77F-156C89658C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D53482E-5EAE-4EBD-AF91-80D16F77B51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RegisterStudent" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="284">
   <si>
     <t>Execute</t>
   </si>
@@ -64,7 +64,7 @@
     <t>Revise</t>
   </si>
   <si>
-    <t>N</t>
+    <t>Y</t>
   </si>
   <si>
     <t>TC2:01</t>
@@ -319,294 +319,294 @@
     <t>MJU6504106396</t>
   </si>
   <si>
+    <t>TC2:22</t>
+  </si>
+  <si>
+    <t>เมาใจ</t>
+  </si>
+  <si>
+    <t>0918079743</t>
+  </si>
+  <si>
+    <t>MJU6504106397</t>
+  </si>
+  <si>
+    <t>TC2:23</t>
+  </si>
+  <si>
+    <t>0918079744</t>
+  </si>
+  <si>
+    <t>MJU6504106398</t>
+  </si>
+  <si>
+    <t>นามสกุลต้องเป็นภาษาไทยหรืออังกฤษ ความยาว 2-85 ตัวอักษร</t>
+  </si>
+  <si>
+    <t>TC2:24</t>
+  </si>
+  <si>
+    <t>จี</t>
+  </si>
+  <si>
+    <t>0918079745</t>
+  </si>
+  <si>
+    <t>MJU6504106399</t>
+  </si>
+  <si>
+    <t>TC2:25</t>
+  </si>
+  <si>
+    <t>จีน</t>
+  </si>
+  <si>
+    <t>0918079746</t>
+  </si>
+  <si>
+    <t>MJU6504106400</t>
+  </si>
+  <si>
+    <t>TC2:26</t>
+  </si>
+  <si>
+    <t>มหาศิริปัญญาโชติวัฒนาสุวรรณ กิตติเพชรบูรณาอุดมเดชสกุลพงศ์ พาณิชย์ศิริวิชยาพรทรัพย์ศิลา</t>
+  </si>
+  <si>
+    <t>0918079747</t>
+  </si>
+  <si>
+    <t>MJU6504106401</t>
+  </si>
+  <si>
+    <t>TC2:27</t>
+  </si>
+  <si>
+    <t>มหาศิริปัญญาโชติวัฒนาสุวรรณ กิตติเพชรบูรณาอุดมเดชสกุลพงศ์ พาณิชย์ศิริวิชยาพรทรัพย์ศิลาก</t>
+  </si>
+  <si>
+    <t>0918079748</t>
+  </si>
+  <si>
+    <t>MJU6504106402</t>
+  </si>
+  <si>
+    <t>TC2:28</t>
+  </si>
+  <si>
+    <t>จ</t>
+  </si>
+  <si>
+    <t>0918079749</t>
+  </si>
+  <si>
+    <t>MJU6504106403</t>
+  </si>
+  <si>
+    <t>TC2:29</t>
+  </si>
+  <si>
+    <t>มหาศิริปัญญาโชติวัฒนาสุวรรณ กิตติเพชรบูรณาอุดมเดชสกุลพงศ์ พาณิชย์ศิริวิชยาพรทรัพย์ศิลากร</t>
+  </si>
+  <si>
+    <t>0918079750</t>
+  </si>
+  <si>
+    <t>MJU6504106404</t>
+  </si>
+  <si>
+    <t>TC2:30</t>
+  </si>
+  <si>
+    <t>จีนดา</t>
+  </si>
+  <si>
+    <t>0918079751</t>
+  </si>
+  <si>
+    <t>MJU6504106405</t>
+  </si>
+  <si>
+    <t>TC2:31</t>
+  </si>
+  <si>
+    <t>จี@</t>
+  </si>
+  <si>
+    <t>0918079752</t>
+  </si>
+  <si>
+    <t>MJU6504106406</t>
+  </si>
+  <si>
+    <t>TC2:32</t>
+  </si>
+  <si>
+    <t>คิม</t>
+  </si>
+  <si>
+    <t>0918079753</t>
+  </si>
+  <si>
+    <t>MJU6504106407</t>
+  </si>
+  <si>
+    <t>TC2:33</t>
+  </si>
+  <si>
+    <t>คิ ม</t>
+  </si>
+  <si>
+    <t>0918079754</t>
+  </si>
+  <si>
+    <t>MJU6504106408</t>
+  </si>
+  <si>
+    <t>TC2:34</t>
+  </si>
+  <si>
+    <t>0918079755</t>
+  </si>
+  <si>
+    <t>MJU6504106409</t>
+  </si>
+  <si>
+    <t>กรุณากรอกนามสกุล</t>
+  </si>
+  <si>
+    <t>TC2:35</t>
+  </si>
+  <si>
+    <t>MJU6504106410</t>
+  </si>
+  <si>
+    <t>TC2:36</t>
+  </si>
+  <si>
+    <t>Eก#9180795</t>
+  </si>
+  <si>
+    <t>MJU6504106411</t>
+  </si>
+  <si>
+    <t>เบอร์โทรต้องขึ้นต้นด้วย 06, 07, 08 หรือ 09 และมี 10 หลักเท่านั้น</t>
+  </si>
+  <si>
+    <t>TC2:37</t>
+  </si>
+  <si>
+    <t>0648581234</t>
+  </si>
+  <si>
+    <t>MJU6504106412</t>
+  </si>
+  <si>
+    <t>TC2:38</t>
+  </si>
+  <si>
+    <t>0748581234</t>
+  </si>
+  <si>
+    <t>MJU6504106413</t>
+  </si>
+  <si>
+    <t>TC2:39</t>
+  </si>
+  <si>
+    <t>0848581234</t>
+  </si>
+  <si>
+    <t>MJU6504106414</t>
+  </si>
+  <si>
+    <t>TC2:40</t>
+  </si>
+  <si>
+    <t>0948581234</t>
+  </si>
+  <si>
+    <t>MJU6504106415</t>
+  </si>
+  <si>
+    <t>TC2:41</t>
+  </si>
+  <si>
+    <t>0719584713</t>
+  </si>
+  <si>
+    <t>MJU6504106416</t>
+  </si>
+  <si>
+    <t>TC2:42</t>
+  </si>
+  <si>
+    <t>0879354033</t>
+  </si>
+  <si>
+    <t>MJU6504106417</t>
+  </si>
+  <si>
+    <t>TC2:43</t>
+  </si>
+  <si>
+    <t>087935403</t>
+  </si>
+  <si>
+    <t>MJU6504106418</t>
+  </si>
+  <si>
+    <t>TC2:44</t>
+  </si>
+  <si>
+    <t>08793540331</t>
+  </si>
+  <si>
+    <t>MJU6504106419</t>
+  </si>
+  <si>
+    <t>TC2:45</t>
+  </si>
+  <si>
+    <t>MJU6504106420</t>
+  </si>
+  <si>
+    <t>TC2:46</t>
+  </si>
+  <si>
+    <t>087 935 4033</t>
+  </si>
+  <si>
+    <t>MJU6504106421</t>
+  </si>
+  <si>
+    <t>เบอร์โทรต้องไม่มีช่องว่าง</t>
+  </si>
+  <si>
+    <t>TC2:47</t>
+  </si>
+  <si>
+    <t>MJU6504106422</t>
+  </si>
+  <si>
+    <t>กรุณากรอกเบอร์โทรศัพท์</t>
+  </si>
+  <si>
+    <t>TC2:48</t>
+  </si>
+  <si>
+    <t>ชั้นปีที่ 1</t>
+  </si>
+  <si>
+    <t>MJU6504106423</t>
+  </si>
+  <si>
+    <t>ลงทะเบียนสำเร็จ</t>
+  </si>
+  <si>
     <t>Fail</t>
   </si>
   <si>
-    <t>TC2:22</t>
-  </si>
-  <si>
-    <t>เมาใจ</t>
-  </si>
-  <si>
-    <t>0918079743</t>
-  </si>
-  <si>
-    <t>MJU6504106397</t>
-  </si>
-  <si>
-    <t>TC2:23</t>
-  </si>
-  <si>
-    <t>0918079744</t>
-  </si>
-  <si>
-    <t>MJU6504106398</t>
-  </si>
-  <si>
-    <t>นามสกุลต้องเป็นภาษาไทยหรืออังกฤษ ความยาว 2-85 ตัวอักษร</t>
-  </si>
-  <si>
-    <t>TC2:24</t>
-  </si>
-  <si>
-    <t>จี</t>
-  </si>
-  <si>
-    <t>0918079745</t>
-  </si>
-  <si>
-    <t>MJU6504106399</t>
-  </si>
-  <si>
-    <t>TC2:25</t>
-  </si>
-  <si>
-    <t>จีน</t>
-  </si>
-  <si>
-    <t>0918079746</t>
-  </si>
-  <si>
-    <t>MJU6504106400</t>
-  </si>
-  <si>
-    <t>TC2:26</t>
-  </si>
-  <si>
-    <t>มหาศิริปัญญาโชติวัฒนาสุวรรณ กิตติเพชรบูรณาอุดมเดชสกุลพงศ์ พาณิชย์ศิริวิชยาพรทรัพย์ศิลา</t>
-  </si>
-  <si>
-    <t>0918079747</t>
-  </si>
-  <si>
-    <t>MJU6504106401</t>
-  </si>
-  <si>
-    <t>TC2:27</t>
-  </si>
-  <si>
-    <t>มหาศิริปัญญาโชติวัฒนาสุวรรณ กิตติเพชรบูรณาอุดมเดชสกุลพงศ์ พาณิชย์ศิริวิชยาพรทรัพย์ศิลาก</t>
-  </si>
-  <si>
-    <t>0918079748</t>
-  </si>
-  <si>
-    <t>MJU6504106402</t>
-  </si>
-  <si>
-    <t>TC2:28</t>
-  </si>
-  <si>
-    <t>จ</t>
-  </si>
-  <si>
-    <t>0918079749</t>
-  </si>
-  <si>
-    <t>MJU6504106403</t>
-  </si>
-  <si>
-    <t>TC2:29</t>
-  </si>
-  <si>
-    <t>มหาศิริปัญญาโชติวัฒนาสุวรรณ กิตติเพชรบูรณาอุดมเดชสกุลพงศ์ พาณิชย์ศิริวิชยาพรทรัพย์ศิลากร</t>
-  </si>
-  <si>
-    <t>0918079750</t>
-  </si>
-  <si>
-    <t>MJU6504106404</t>
-  </si>
-  <si>
-    <t>TC2:30</t>
-  </si>
-  <si>
-    <t>จีนดา</t>
-  </si>
-  <si>
-    <t>0918079751</t>
-  </si>
-  <si>
-    <t>MJU6504106405</t>
-  </si>
-  <si>
-    <t>TC2:31</t>
-  </si>
-  <si>
-    <t>จี@</t>
-  </si>
-  <si>
-    <t>0918079752</t>
-  </si>
-  <si>
-    <t>MJU6504106406</t>
-  </si>
-  <si>
-    <t>TC2:32</t>
-  </si>
-  <si>
-    <t>คิม</t>
-  </si>
-  <si>
-    <t>0918079753</t>
-  </si>
-  <si>
-    <t>MJU6504106407</t>
-  </si>
-  <si>
-    <t>TC2:33</t>
-  </si>
-  <si>
-    <t>คิ ม</t>
-  </si>
-  <si>
-    <t>0918079754</t>
-  </si>
-  <si>
-    <t>MJU6504106408</t>
-  </si>
-  <si>
-    <t>TC2:34</t>
-  </si>
-  <si>
-    <t>0918079755</t>
-  </si>
-  <si>
-    <t>MJU6504106409</t>
-  </si>
-  <si>
-    <t>กรุณากรอกนามสกุล</t>
-  </si>
-  <si>
-    <t>TC2:35</t>
-  </si>
-  <si>
-    <t>MJU6504106410</t>
-  </si>
-  <si>
-    <t>TC2:36</t>
-  </si>
-  <si>
-    <t>Eก#9180795</t>
-  </si>
-  <si>
-    <t>MJU6504106411</t>
-  </si>
-  <si>
-    <t>เบอร์โทรต้องขึ้นต้นด้วย 06, 07, 08 หรือ 09 และมี 10 หลักเท่านั้น</t>
-  </si>
-  <si>
-    <t>TC2:37</t>
-  </si>
-  <si>
-    <t>0648581234</t>
-  </si>
-  <si>
-    <t>MJU6504106412</t>
-  </si>
-  <si>
-    <t>TC2:38</t>
-  </si>
-  <si>
-    <t>0748581234</t>
-  </si>
-  <si>
-    <t>MJU6504106413</t>
-  </si>
-  <si>
-    <t>TC2:39</t>
-  </si>
-  <si>
-    <t>0848581234</t>
-  </si>
-  <si>
-    <t>MJU6504106414</t>
-  </si>
-  <si>
-    <t>TC2:40</t>
-  </si>
-  <si>
-    <t>0948581234</t>
-  </si>
-  <si>
-    <t>MJU6504106415</t>
-  </si>
-  <si>
-    <t>TC2:41</t>
-  </si>
-  <si>
-    <t>0719584713</t>
-  </si>
-  <si>
-    <t>MJU6504106416</t>
-  </si>
-  <si>
-    <t>TC2:42</t>
-  </si>
-  <si>
-    <t>0879354033</t>
-  </si>
-  <si>
-    <t>MJU6504106417</t>
-  </si>
-  <si>
-    <t>TC2:43</t>
-  </si>
-  <si>
-    <t>087935403</t>
-  </si>
-  <si>
-    <t>MJU6504106418</t>
-  </si>
-  <si>
-    <t>TC2:44</t>
-  </si>
-  <si>
-    <t>08793540331</t>
-  </si>
-  <si>
-    <t>MJU6504106419</t>
-  </si>
-  <si>
-    <t>TC2:45</t>
-  </si>
-  <si>
-    <t>MJU6504106420</t>
-  </si>
-  <si>
-    <t>TC2:46</t>
-  </si>
-  <si>
-    <t>087 935 4033</t>
-  </si>
-  <si>
-    <t>MJU6504106421</t>
-  </si>
-  <si>
-    <t>เบอร์โทรต้องไม่มีช่องว่าง</t>
-  </si>
-  <si>
-    <t>TC2:47</t>
-  </si>
-  <si>
-    <t>MJU6504106422</t>
-  </si>
-  <si>
-    <t>กรุณากรอกเบอร์โทรศัพท์</t>
-  </si>
-  <si>
-    <t>TC2:48</t>
-  </si>
-  <si>
-    <t>ชั้นปีที่ 1</t>
-  </si>
-  <si>
-    <t>MJU6504106423</t>
-  </si>
-  <si>
-    <t>ลงทะเบียนสำเร็จ</t>
-  </si>
-  <si>
     <t>TC2:49</t>
   </si>
   <si>
@@ -673,16 +673,13 @@
     <t>MJU 650410640</t>
   </si>
   <si>
-    <t>กรุณากรอกโดยห้ามมีช่องว่าง</t>
-  </si>
-  <si>
     <t>ห้ามมีช่องว่างในอีเมล</t>
   </si>
   <si>
     <t>TC2:57</t>
   </si>
   <si>
-    <t>mju6504106400</t>
+    <t>mju6504106435</t>
   </si>
   <si>
     <t>TC2:58</t>
@@ -691,9 +688,6 @@
     <t>mju650410640</t>
   </si>
   <si>
-    <t>กรุณากรอกความยาวให้มีขนาด 13 ตัวพอดี</t>
-  </si>
-  <si>
     <t>TC2:59</t>
   </si>
   <si>
@@ -701,9 +695,6 @@
   </si>
   <si>
     <t>TC2:60</t>
-  </si>
-  <si>
-    <t>กรุณากรอกอีเมล์รูปแบบของอีเมล MJU</t>
   </si>
   <si>
     <t>กรุณากรอกอีเมล</t>
@@ -1282,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="H44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2219,7 +2210,7 @@
         <v>23</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N22" s="12"/>
     </row>
@@ -2228,7 +2219,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C23" s="3">
         <v>6504106397</v>
@@ -2237,17 +2228,17 @@
         <v>16</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="G23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="I23" s="10" t="s">
         <v>21</v>
       </c>
@@ -2261,7 +2252,7 @@
         <v>23</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N23" s="12"/>
     </row>
@@ -2270,7 +2261,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C24" s="3">
         <v>6504106398</v>
@@ -2282,28 +2273,28 @@
         <v>1234</v>
       </c>
       <c r="F24" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I24" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="L24" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N24" s="12"/>
     </row>
@@ -2312,7 +2303,7 @@
         <v>14</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C25" s="3">
         <v>6504106399</v>
@@ -2321,17 +2312,17 @@
         <v>16</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="G25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>111</v>
-      </c>
       <c r="I25" s="10" t="s">
         <v>21</v>
       </c>
@@ -2345,7 +2336,7 @@
         <v>23</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N25" s="12"/>
     </row>
@@ -2354,7 +2345,7 @@
         <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C26" s="3">
         <v>6504106400</v>
@@ -2363,17 +2354,17 @@
         <v>16</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="G26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="15" t="s">
-        <v>115</v>
-      </c>
       <c r="I26" s="10" t="s">
         <v>21</v>
       </c>
@@ -2387,7 +2378,7 @@
         <v>23</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N26" s="12"/>
     </row>
@@ -2396,7 +2387,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C27" s="3">
         <v>6504106401</v>
@@ -2405,17 +2396,17 @@
         <v>16</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="G27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="15" t="s">
-        <v>119</v>
-      </c>
       <c r="I27" s="10" t="s">
         <v>21</v>
       </c>
@@ -2423,13 +2414,13 @@
         <v>22</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N27" s="12"/>
     </row>
@@ -2438,7 +2429,7 @@
         <v>14</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C28" s="3">
         <v>6504106402</v>
@@ -2447,17 +2438,17 @@
         <v>16</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="G28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H28" s="15" t="s">
-        <v>123</v>
-      </c>
       <c r="I28" s="10" t="s">
         <v>21</v>
       </c>
@@ -2465,13 +2456,13 @@
         <v>22</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N28" s="12"/>
     </row>
@@ -2480,7 +2471,7 @@
         <v>14</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C29" s="3">
         <v>6504106403</v>
@@ -2489,17 +2480,17 @@
         <v>16</v>
       </c>
       <c r="E29" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="G29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H29" s="15" t="s">
-        <v>127</v>
-      </c>
       <c r="I29" s="10" t="s">
         <v>21</v>
       </c>
@@ -2507,13 +2498,13 @@
         <v>22</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N29" s="12"/>
     </row>
@@ -2522,7 +2513,7 @@
         <v>14</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C30" s="3">
         <v>6504106404</v>
@@ -2531,17 +2522,17 @@
         <v>16</v>
       </c>
       <c r="E30" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="G30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>131</v>
-      </c>
       <c r="I30" s="10" t="s">
         <v>21</v>
       </c>
@@ -2549,13 +2540,13 @@
         <v>22</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N30" s="12"/>
     </row>
@@ -2564,7 +2555,7 @@
         <v>14</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C31" s="3">
         <v>6504106405</v>
@@ -2573,17 +2564,17 @@
         <v>16</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="G31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>135</v>
-      </c>
       <c r="I31" s="10" t="s">
         <v>21</v>
       </c>
@@ -2597,7 +2588,7 @@
         <v>23</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N31" s="12"/>
     </row>
@@ -2606,7 +2597,7 @@
         <v>14</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C32" s="3">
         <v>6504106406</v>
@@ -2615,17 +2606,17 @@
         <v>16</v>
       </c>
       <c r="E32" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="G32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H32" s="15" t="s">
-        <v>139</v>
-      </c>
       <c r="I32" s="10" t="s">
         <v>21</v>
       </c>
@@ -2633,13 +2624,13 @@
         <v>22</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N32" s="12"/>
     </row>
@@ -2648,7 +2639,7 @@
         <v>14</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C33" s="3">
         <v>6504106407</v>
@@ -2657,17 +2648,17 @@
         <v>16</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="G33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>143</v>
-      </c>
       <c r="I33" s="10" t="s">
         <v>21</v>
       </c>
@@ -2681,7 +2672,7 @@
         <v>23</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N33" s="12"/>
     </row>
@@ -2690,7 +2681,7 @@
         <v>14</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C34" s="3">
         <v>6504106408</v>
@@ -2699,17 +2690,17 @@
         <v>16</v>
       </c>
       <c r="E34" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F34" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="G34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>147</v>
-      </c>
       <c r="I34" s="10" t="s">
         <v>21</v>
       </c>
@@ -2723,7 +2714,7 @@
         <v>23</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N34" s="12"/>
     </row>
@@ -2732,7 +2723,7 @@
         <v>14</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C35" s="3">
         <v>6504106409</v>
@@ -2742,25 +2733,25 @@
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" s="15" t="s">
+      <c r="I35" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="I35" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="L35" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>24</v>
@@ -2772,7 +2763,7 @@
         <v>14</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C36" s="3">
         <v>6504106410</v>
@@ -2790,7 +2781,7 @@
         <v>19</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I36" s="10" t="s">
         <v>21</v>
@@ -2805,7 +2796,7 @@
         <v>23</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N36" s="12"/>
     </row>
@@ -2814,7 +2805,7 @@
         <v>14</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C37" s="3">
         <v>6504106411</v>
@@ -2826,28 +2817,28 @@
         <v>17</v>
       </c>
       <c r="F37" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="15" t="s">
+      <c r="I37" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K37" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="I37" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="L37" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N37" s="12"/>
     </row>
@@ -2856,7 +2847,7 @@
         <v>14</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C38" s="3">
         <v>6504106412</v>
@@ -2868,14 +2859,14 @@
         <v>17</v>
       </c>
       <c r="F38" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>160</v>
-      </c>
       <c r="I38" s="10" t="s">
         <v>21</v>
       </c>
@@ -2889,7 +2880,7 @@
         <v>23</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N38" s="12"/>
     </row>
@@ -2898,7 +2889,7 @@
         <v>14</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C39" s="3">
         <v>6504106413</v>
@@ -2910,14 +2901,14 @@
         <v>17</v>
       </c>
       <c r="F39" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>163</v>
-      </c>
       <c r="I39" s="10" t="s">
         <v>21</v>
       </c>
@@ -2931,7 +2922,7 @@
         <v>23</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N39" s="12"/>
     </row>
@@ -2940,7 +2931,7 @@
         <v>14</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C40" s="3">
         <v>6504106414</v>
@@ -2952,14 +2943,14 @@
         <v>17</v>
       </c>
       <c r="F40" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H40" s="15" t="s">
-        <v>166</v>
-      </c>
       <c r="I40" s="10" t="s">
         <v>21</v>
       </c>
@@ -2973,7 +2964,7 @@
         <v>23</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N40" s="12"/>
     </row>
@@ -2982,7 +2973,7 @@
         <v>14</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C41" s="3">
         <v>6504106415</v>
@@ -2994,14 +2985,14 @@
         <v>17</v>
       </c>
       <c r="F41" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H41" s="15" t="s">
-        <v>169</v>
-      </c>
       <c r="I41" s="10" t="s">
         <v>21</v>
       </c>
@@ -3015,7 +3006,7 @@
         <v>23</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N41" s="12"/>
     </row>
@@ -3024,7 +3015,7 @@
         <v>14</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C42" s="3">
         <v>6504106416</v>
@@ -3036,14 +3027,14 @@
         <v>17</v>
       </c>
       <c r="F42" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H42" s="15" t="s">
-        <v>172</v>
-      </c>
       <c r="I42" s="10" t="s">
         <v>21</v>
       </c>
@@ -3057,7 +3048,7 @@
         <v>23</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N42" s="12"/>
     </row>
@@ -3066,7 +3057,7 @@
         <v>14</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C43" s="3">
         <v>6504106417</v>
@@ -3078,14 +3069,14 @@
         <v>17</v>
       </c>
       <c r="F43" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H43" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>175</v>
-      </c>
       <c r="I43" s="10" t="s">
         <v>21</v>
       </c>
@@ -3099,7 +3090,7 @@
         <v>23</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N43" s="12"/>
     </row>
@@ -3108,7 +3099,7 @@
         <v>14</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C44" s="3">
         <v>6504106418</v>
@@ -3120,14 +3111,14 @@
         <v>17</v>
       </c>
       <c r="F44" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>178</v>
-      </c>
       <c r="I44" s="10" t="s">
         <v>21</v>
       </c>
@@ -3135,13 +3126,13 @@
         <v>22</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N44" s="12"/>
     </row>
@@ -3150,7 +3141,7 @@
         <v>14</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C45" s="3">
         <v>6504106419</v>
@@ -3162,14 +3153,14 @@
         <v>17</v>
       </c>
       <c r="F45" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H45" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="G45" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H45" s="15" t="s">
-        <v>181</v>
-      </c>
       <c r="I45" s="10" t="s">
         <v>21</v>
       </c>
@@ -3177,13 +3168,13 @@
         <v>22</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N45" s="12"/>
     </row>
@@ -3192,7 +3183,7 @@
         <v>14</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C46" s="3">
         <v>6504106420</v>
@@ -3204,13 +3195,13 @@
         <v>17</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I46" s="10" t="s">
         <v>21</v>
@@ -3225,7 +3216,7 @@
         <v>23</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N46" s="12"/>
     </row>
@@ -3234,7 +3225,7 @@
         <v>14</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C47" s="3">
         <v>6504106421</v>
@@ -3246,28 +3237,28 @@
         <v>17</v>
       </c>
       <c r="F47" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H47" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H47" s="15" t="s">
+      <c r="I47" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K47" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="I47" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="L47" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N47" s="12"/>
     </row>
@@ -3276,7 +3267,7 @@
         <v>14</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C48" s="3">
         <v>6504106422</v>
@@ -3292,22 +3283,22 @@
         <v>19</v>
       </c>
       <c r="H48" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K48" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="I48" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="L48" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N48" s="12"/>
     </row>
@@ -3316,7 +3307,7 @@
         <v>14</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C49" s="3">
         <v>6504106423</v>
@@ -3331,11 +3322,11 @@
         <v>18</v>
       </c>
       <c r="G49" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="H49" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="H49" s="15" t="s">
-        <v>193</v>
-      </c>
       <c r="I49" s="10" t="s">
         <v>21</v>
       </c>
@@ -3343,13 +3334,13 @@
         <v>22</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>194</v>
+        <v>23</v>
       </c>
       <c r="L49" s="2" t="s">
         <v>23</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N49" s="12"/>
     </row>
@@ -3385,13 +3376,13 @@
         <v>22</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>194</v>
+        <v>23</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>23</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N50" s="12"/>
     </row>
@@ -3427,13 +3418,13 @@
         <v>22</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>194</v>
+        <v>23</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>23</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N51" s="12"/>
     </row>
@@ -3469,13 +3460,13 @@
         <v>22</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>194</v>
+        <v>23</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>23</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N52" s="12"/>
     </row>
@@ -3553,13 +3544,13 @@
         <v>22</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>194</v>
+        <v>23</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>23</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N54" s="12"/>
     </row>
@@ -3601,7 +3592,7 @@
         <v>212</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>99</v>
+        <v>194</v>
       </c>
       <c r="N55" s="12"/>
     </row>
@@ -3637,13 +3628,13 @@
         <v>22</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>194</v>
+        <v>23</v>
       </c>
       <c r="L56" s="2" t="s">
         <v>23</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N56" s="12"/>
     </row>
@@ -3682,10 +3673,10 @@
         <v>217</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N57" s="12"/>
     </row>
@@ -3694,7 +3685,7 @@
         <v>14</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C58" s="3">
         <v>6504106432</v>
@@ -3712,7 +3703,7 @@
         <v>19</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I58" s="10" t="s">
         <v>21</v>
@@ -3721,13 +3712,13 @@
         <v>22</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>194</v>
+        <v>23</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N58" s="12"/>
     </row>
@@ -3736,7 +3727,7 @@
         <v>14</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C59" s="3">
         <v>6504106433</v>
@@ -3754,7 +3745,7 @@
         <v>19</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I59" s="10" t="s">
         <v>21</v>
@@ -3763,13 +3754,13 @@
         <v>22</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>212</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N59" s="12"/>
     </row>
@@ -3778,7 +3769,7 @@
         <v>14</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C60" s="3">
         <v>6504106434</v>
@@ -3796,7 +3787,7 @@
         <v>19</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I60" s="10" t="s">
         <v>21</v>
@@ -3805,13 +3796,13 @@
         <v>22</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="L60" s="2" t="s">
         <v>212</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N60" s="12"/>
     </row>
@@ -3820,7 +3811,7 @@
         <v>14</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C61" s="3">
         <v>6504106435</v>
@@ -3845,13 +3836,13 @@
         <v>22</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N61" s="12"/>
     </row>
@@ -3860,7 +3851,7 @@
         <v>14</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C62" s="3">
         <v>6504106436</v>
@@ -3878,7 +3869,7 @@
         <v>19</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="I62" s="10" t="s">
         <v>21</v>
@@ -3887,13 +3878,13 @@
         <v>22</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>194</v>
+        <v>23</v>
       </c>
       <c r="L62" s="2" t="s">
         <v>23</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N62" s="12"/>
     </row>
@@ -3902,7 +3893,7 @@
         <v>14</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C63" s="3">
         <v>6504106437</v>
@@ -3920,22 +3911,22 @@
         <v>19</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N63" s="12"/>
     </row>
@@ -3944,7 +3935,7 @@
         <v>14</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C64" s="3">
         <v>6504106438</v>
@@ -3962,10 +3953,10 @@
         <v>19</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I64" s="10" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>22</v>
@@ -3977,7 +3968,7 @@
         <v>23</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N64" s="12"/>
     </row>
@@ -3986,7 +3977,7 @@
         <v>14</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C65" s="3">
         <v>6504106439</v>
@@ -4004,10 +3995,10 @@
         <v>19</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>22</v>
@@ -4019,7 +4010,7 @@
         <v>23</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N65" s="12"/>
     </row>
@@ -4028,7 +4019,7 @@
         <v>14</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C66" s="3">
         <v>6504106440</v>
@@ -4046,10 +4037,10 @@
         <v>19</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>22</v>
@@ -4061,7 +4052,7 @@
         <v>23</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N66" s="12"/>
     </row>
@@ -4070,7 +4061,7 @@
         <v>14</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C67" s="3">
         <v>6504106441</v>
@@ -4088,10 +4079,10 @@
         <v>19</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="I67" s="10" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>22</v>
@@ -4103,7 +4094,7 @@
         <v>23</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N67" s="12"/>
     </row>
@@ -4112,7 +4103,7 @@
         <v>14</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C68" s="3">
         <v>6504106442</v>
@@ -4130,22 +4121,22 @@
         <v>19</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N68" s="12"/>
     </row>
@@ -4154,7 +4145,7 @@
         <v>14</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C69" s="3">
         <v>6504106443</v>
@@ -4172,22 +4163,22 @@
         <v>19</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="I69" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N69" s="12"/>
     </row>
@@ -4196,7 +4187,7 @@
         <v>14</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C70" s="3">
         <v>6504106444</v>
@@ -4208,13 +4199,13 @@
         <v>17</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="I70" s="10" t="s">
         <v>21</v>
@@ -4229,7 +4220,7 @@
         <v>23</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N70" s="12"/>
     </row>
@@ -4238,7 +4229,7 @@
         <v>14</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C71" s="3">
         <v>6504106445</v>
@@ -4250,16 +4241,16 @@
         <v>17</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="I71" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>22</v>
@@ -4271,7 +4262,7 @@
         <v>23</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N71" s="12"/>
     </row>
@@ -4280,7 +4271,7 @@
         <v>14</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C72" s="3">
         <v>6504106446</v>
@@ -4292,16 +4283,16 @@
         <v>17</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="I72" s="10" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>22</v>
@@ -4313,7 +4304,7 @@
         <v>23</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N72" s="12"/>
     </row>
@@ -4322,7 +4313,7 @@
         <v>14</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C73" s="3">
         <v>6504106447</v>
@@ -4334,28 +4325,28 @@
         <v>17</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I73" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="M73" s="2" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N73" s="12"/>
     </row>
@@ -4364,7 +4355,7 @@
         <v>14</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C74" s="3">
         <v>6504106448</v>
@@ -4376,23 +4367,23 @@
         <v>17</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I74" s="11"/>
       <c r="J74" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="M74" s="2" t="s">
         <v>24</v>
@@ -4404,7 +4395,7 @@
         <v>14</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C75" s="3">
         <v>6504106449</v>
@@ -4416,13 +4407,13 @@
         <v>17</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I75" s="10" t="s">
         <v>21</v>
@@ -4431,13 +4422,13 @@
         <v>22</v>
       </c>
       <c r="K75" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M75" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="L75" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M75" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="N75" s="12"/>
     </row>
@@ -4446,7 +4437,7 @@
         <v>14</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C76" s="3">
         <v>6504106450</v>
@@ -4458,28 +4449,28 @@
         <v>17</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="I76" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J76" s="6" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="L76" s="2" t="s">
         <v>23</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>99</v>
+        <v>194</v>
       </c>
       <c r="N76" s="12"/>
     </row>
@@ -4488,7 +4479,7 @@
         <v>14</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C77" s="3">
         <v>6504106451</v>
@@ -4500,28 +4491,28 @@
         <v>17</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="I77" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="K77" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M77" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="L77" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M77" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="N77" s="12"/>
     </row>
@@ -4530,7 +4521,7 @@
         <v>14</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C78" s="3">
         <v>6504106452</v>
@@ -4542,28 +4533,28 @@
         <v>17</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I78" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="K78" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L78" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M78" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="L78" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M78" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="N78" s="12"/>
     </row>
@@ -4572,7 +4563,7 @@
         <v>14</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C79" s="3">
         <v>6504106453</v>
@@ -4584,28 +4575,28 @@
         <v>17</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="I79" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J79" s="7" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="L79" s="2" t="s">
         <v>23</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>99</v>
+        <v>194</v>
       </c>
       <c r="N79" s="12"/>
     </row>
@@ -4614,7 +4605,7 @@
         <v>14</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C80" s="3">
         <v>6504106454</v>
@@ -4626,26 +4617,26 @@
         <v>17</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I80" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J80" s="11"/>
       <c r="K80" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="L80" s="2" t="s">
         <v>23</v>
       </c>
       <c r="M80" s="2" t="s">
-        <v>99</v>
+        <v>194</v>
       </c>
       <c r="N80" s="12"/>
     </row>

</xml_diff>